<commit_message>
fix: drop datasets cant be run
</commit_message>
<xml_diff>
--- a/docs/acc.xlsx
+++ b/docs/acc.xlsx
@@ -437,7 +437,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>测试时间:  : 2025-11-05 17:09:41</t>
+          <t>测试时间:  : 2025-11-07 13:54:00</t>
         </is>
       </c>
     </row>
@@ -550,22 +550,67 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>Qwen3-0.6B</t>
+          <t>Qwen3-4B-Instruct-2507</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>0.3763 ± 0.0048</t>
+          <t>0.3871 ± 0.0049</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>0.4744 ± 0.0050</t>
+          <t>0.4345 ± 0.0049</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>109.60S</t>
+          <t>241.51S</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t>0.3878 ± 0.0049</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>0.4352 ± 0.0049</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>293.21S</t>
+        </is>
+      </c>
+      <c r="I5" s="1" t="inlineStr">
+        <is>
+          <t>0.3889 ± 0.0049</t>
+        </is>
+      </c>
+      <c r="J5" s="1" t="inlineStr">
+        <is>
+          <t>0.4362 ± 0.0049</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr">
+        <is>
+          <t>236.85S</t>
+        </is>
+      </c>
+      <c r="L5" s="1" t="inlineStr">
+        <is>
+          <t>0.3878 ± 0.0049</t>
+        </is>
+      </c>
+      <c r="M5" s="1" t="inlineStr">
+        <is>
+          <t>0.4349 ± 0.0049</t>
+        </is>
+      </c>
+      <c r="N5" s="1" t="inlineStr">
+        <is>
+          <t>275.39S</t>
         </is>
       </c>
     </row>

</xml_diff>